<commit_message>
LED holder, light list update, netlist update
</commit_message>
<xml_diff>
--- a/ChartLights/lightlist/lightSort.xlsx
+++ b/ChartLights/lightlist/lightSort.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17331"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20484" windowHeight="15360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="3" r:id="rId1"/>
@@ -1449,10 +1449,10 @@
     <t>Label</t>
   </si>
   <si>
-    <t>Driftmier</t>
-  </si>
-  <si>
-    <t>VaLeighGirl</t>
+    <t>Fl B M Drifmier</t>
+  </si>
+  <si>
+    <t>Bl B M VaLeighGirl</t>
   </si>
 </sst>
 </file>
@@ -2067,7 +2067,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0FAF610D-B4ED-416E-8850-0AAFD1908285}" type="CELLRANGE">
+                    <a:fld id="{AD036804-D714-469A-8B60-5FDBBB32DFD8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2100,7 +2100,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA945C66-B32B-4FF9-9DFA-1E7AAD77052A}" type="CELLRANGE">
+                    <a:fld id="{3E072522-2C2E-4F10-8C88-0998ED13AF9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2133,7 +2133,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64D15338-FB99-453A-8C5C-6BCEB9639461}" type="CELLRANGE">
+                    <a:fld id="{9B891318-3EB4-440F-8A3D-E01EEB106A5D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2166,7 +2166,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB28CD25-FCBD-4964-AAA1-A70EEC8D9CAB}" type="CELLRANGE">
+                    <a:fld id="{B780922A-82D4-4297-9071-C31B90AD8F5C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2199,7 +2199,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23388B2A-2CC1-45A2-AEBB-09EA50F0D9AC}" type="CELLRANGE">
+                    <a:fld id="{CFD50CE3-330C-4407-BD1F-C7277E544F6F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2232,7 +2232,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DB759DCD-A049-4319-B902-1F564E1B1288}" type="CELLRANGE">
+                    <a:fld id="{D6EF1743-3650-4D2A-BC6F-CFACE6B0BD44}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2265,7 +2265,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D218F06F-3156-4282-97E1-B6BEE75A2388}" type="CELLRANGE">
+                    <a:fld id="{7AED962F-19E4-4785-B4F7-8D3640AB4568}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2298,7 +2298,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9DAECC74-E0E0-44D0-8A37-2B3014C6EBC3}" type="CELLRANGE">
+                    <a:fld id="{F2E10B3B-5C98-4A1D-8817-4FEA84DBD013}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2331,7 +2331,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91DA228F-84B4-456D-A690-5099621370BD}" type="CELLRANGE">
+                    <a:fld id="{E0BDC412-30C7-46DF-8128-A994107FE979}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2364,7 +2364,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD982857-98D7-4CF2-B796-EA2B42DEC49E}" type="CELLRANGE">
+                    <a:fld id="{87D246E8-19E3-458C-986A-0269FE738A30}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2397,7 +2397,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B1B2676-0EFB-4B97-B434-AFE5C6FE3746}" type="CELLRANGE">
+                    <a:fld id="{766ECBA6-464C-46E3-89F5-5E69B5A6293A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2430,7 +2430,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8713C223-4767-417B-916E-EDF96DC592CE}" type="CELLRANGE">
+                    <a:fld id="{10CDAA7E-E869-4709-B1D1-E2F7BF9C0292}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2463,7 +2463,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D49E98D4-48A4-4B3D-A52F-C2BEB645BBB4}" type="CELLRANGE">
+                    <a:fld id="{5389B741-30C1-4DCE-8269-0ED7470CC835}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2496,7 +2496,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D6933973-CF04-4192-8A17-DC3BEAB2D87F}" type="CELLRANGE">
+                    <a:fld id="{956C7BF9-C984-4766-83FE-3C8E736B0120}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2529,7 +2529,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{759EDC3B-23B5-473C-9588-F7D5484798F1}" type="CELLRANGE">
+                    <a:fld id="{D0533C22-9134-4AD9-8584-EBB21AB001EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2562,7 +2562,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{115C3D37-75A0-463E-9919-8A19CFE461D5}" type="CELLRANGE">
+                    <a:fld id="{1C239527-57B4-4845-B8AA-C199627B3883}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2595,7 +2595,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{818F12D4-DB2F-4D5D-AE5A-43B063AB2613}" type="CELLRANGE">
+                    <a:fld id="{E0DD58BA-B094-4B5C-957A-0E29122AC11A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2628,7 +2628,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{414457BE-4DFC-4654-AD4C-1613FDB141CE}" type="CELLRANGE">
+                    <a:fld id="{A60B7E94-4728-42EE-9838-605610A9320A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2661,7 +2661,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21C4A93E-EA68-47E8-97D5-BBD09576525D}" type="CELLRANGE">
+                    <a:fld id="{8A2C29F3-16C0-4509-A6CB-39A30BB0A574}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2694,7 +2694,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A8CA417D-94EE-4642-A75D-3D0D8347FA47}" type="CELLRANGE">
+                    <a:fld id="{8AA3D95E-1EA2-432D-AE9E-338B04833B68}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2727,7 +2727,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D245C060-8EE2-413E-8770-0B665A92B1E2}" type="CELLRANGE">
+                    <a:fld id="{DEF5E347-8460-4AAD-A366-0FBE571BC0B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2760,7 +2760,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3123546-67CB-4D11-9FDC-61EECCE87E0F}" type="CELLRANGE">
+                    <a:fld id="{5E4C9572-5746-499F-B5DA-A9834ABF8175}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2793,7 +2793,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A4A3914F-64AB-4CD4-902B-29489933A6E3}" type="CELLRANGE">
+                    <a:fld id="{1B68663D-37DF-4FD0-A901-83C3858EC5F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2826,7 +2826,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DBB33D08-BB21-42C1-8A10-04D944B6482E}" type="CELLRANGE">
+                    <a:fld id="{808C9B42-738B-4F05-B619-DAE353B1C00F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2859,7 +2859,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1147BD8C-39AD-428E-82EB-BC9E4A6A89F9}" type="CELLRANGE">
+                    <a:fld id="{50F7BADA-8F82-449C-9BA4-4D0B38255568}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2892,7 +2892,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60E50897-6BA2-43D4-B095-50DBF78335A9}" type="CELLRANGE">
+                    <a:fld id="{AD663955-B8BB-4362-ADCD-F63F8689D13A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2925,7 +2925,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{131F37B0-C48E-4508-A982-BF8D52AA42C7}" type="CELLRANGE">
+                    <a:fld id="{829507CF-A817-47A3-AB1C-F14B76EED890}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2958,7 +2958,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A715D2B9-3FF5-4C73-BE25-2AC0D69CDFBC}" type="CELLRANGE">
+                    <a:fld id="{FC494693-7155-43F3-96B3-8F762D493AE3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2991,7 +2991,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BE237FA-0126-48A1-9256-4C9A117CF8C9}" type="CELLRANGE">
+                    <a:fld id="{F60CC22B-F717-413D-8A37-FFF4D9B02C3F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3024,7 +3024,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27A31118-7DB6-4198-A9E6-9DAA71E1F5AD}" type="CELLRANGE">
+                    <a:fld id="{BB9809FA-B5FB-441B-B70E-60B47F25B413}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3057,7 +3057,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2415D30-B86F-47C3-A1D3-EE7707513AF9}" type="CELLRANGE">
+                    <a:fld id="{B9617BFE-E5DB-423A-AFF1-095197AD49D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3090,7 +3090,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9FD9035D-58C6-441E-A6D9-1DBFB8A6178D}" type="CELLRANGE">
+                    <a:fld id="{5B8BAB5E-3DDB-4730-B087-C8058E9D8BAE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3123,7 +3123,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{38457D2D-DF35-4FE7-9921-F7868BEAA72F}" type="CELLRANGE">
+                    <a:fld id="{704C542E-A588-4DA5-B9A5-3AA1678862BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3156,7 +3156,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9EA499F-32F7-4F9E-B6AA-D03378F3AE10}" type="CELLRANGE">
+                    <a:fld id="{0CA3331B-9AEF-49A6-9D63-C8B3B3EF552D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3189,7 +3189,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42FF4718-ED89-4D85-95DE-3824F0764326}" type="CELLRANGE">
+                    <a:fld id="{353CC10C-EDA2-4786-95B7-4EC311A342B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3222,7 +3222,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A37C0252-1632-4D83-B84B-01FAC0FA8C17}" type="CELLRANGE">
+                    <a:fld id="{51F519C3-7945-4ACD-9638-5C6ECD2D1F6E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3255,7 +3255,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B311B4CD-7EC1-47C5-B722-E99893E73417}" type="CELLRANGE">
+                    <a:fld id="{7A5B9003-AC08-4554-8EA3-B878CD6C0285}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3288,7 +3288,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8217026D-A4A5-4F25-B362-667F7B185F3B}" type="CELLRANGE">
+                    <a:fld id="{0A07AA38-2FCB-4503-AACC-9A4F0E6ECAC1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3321,7 +3321,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3203868-E665-438B-92F1-11D21C108DD5}" type="CELLRANGE">
+                    <a:fld id="{D0407D95-0504-4225-BF0D-8A4A7C7F8D4F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3354,7 +3354,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C814D77-7C1D-44A4-841D-27BBFAD53131}" type="CELLRANGE">
+                    <a:fld id="{BB261AA0-5ADA-4F04-8A84-49DBB6D21CB7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3703,10 +3703,10 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="131"/>
                   <c:pt idx="0">
-                    <c:v>1: Driftmier</c:v>
+                    <c:v>1: Fl B M Drifmier</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2: VaLeighGirl</c:v>
+                    <c:v>2: Bl B M VaLeighGirl</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>3: Fl W 5s</c:v>
@@ -4838,7 +4838,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="266" workbookViewId="0"/>
+    <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4849,7 +4849,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656320" cy="6281420"/>
+    <xdr:ext cx="8669182" cy="6295094"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5216,32 +5216,32 @@
   </sheetPr>
   <dimension ref="A1:W133"/>
   <sheetViews>
-    <sheetView topLeftCell="M3" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4:V133"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="26.44140625" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="34.44140625" customWidth="1"/>
-    <col min="12" max="12" width="35.77734375" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" customWidth="1"/>
-    <col min="14" max="14" width="26.109375" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" customWidth="1"/>
-    <col min="19" max="19" width="9.109375" customWidth="1"/>
-    <col min="20" max="20" width="28.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.375" customWidth="1"/>
+    <col min="9" max="9" width="26.5" customWidth="1"/>
+    <col min="10" max="10" width="15.375" customWidth="1"/>
+    <col min="11" max="11" width="34.5" customWidth="1"/>
+    <col min="12" max="12" width="35.75" customWidth="1"/>
+    <col min="13" max="13" width="12.75" customWidth="1"/>
+    <col min="14" max="14" width="26.125" customWidth="1"/>
+    <col min="17" max="17" width="9.125" customWidth="1"/>
+    <col min="18" max="18" width="9.625" customWidth="1"/>
+    <col min="19" max="19" width="9.125" customWidth="1"/>
+    <col min="20" max="20" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5312,12 +5312,18 @@
         <v>472</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>38.976108000000004</v>
       </c>
       <c r="C3">
         <v>76.499307000000002</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
       </c>
       <c r="N3" t="s">
         <v>473</v>
@@ -5328,15 +5334,21 @@
       </c>
       <c r="W3" s="1" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Count]],": ",Table1[[#This Row],[Characteristic]])</f>
-        <v>1: Driftmier</v>
+        <v>1: Fl B M Drifmier</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>38.772939999999998</v>
       </c>
       <c r="C4">
         <v>76.563226999999998</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
       </c>
       <c r="N4" t="s">
         <v>474</v>
@@ -5347,10 +5359,10 @@
       </c>
       <c r="W4" s="1" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Count]],": ",Table1[[#This Row],[Characteristic]])</f>
-        <v>2: VaLeighGirl</v>
+        <v>2: Bl B M VaLeighGirl</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>16</v>
       </c>
@@ -5414,7 +5426,7 @@
         <v>3: Fl W 5s</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9</v>
       </c>
@@ -5478,7 +5490,7 @@
         <v>4: Fl W 6s</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9</v>
       </c>
@@ -5542,7 +5554,7 @@
         <v>5: Fl W 6s</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -5603,7 +5615,7 @@
         <v>6: Fl W 6s</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -5664,7 +5676,7 @@
         <v>7: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -5725,7 +5737,7 @@
         <v>8: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -5786,7 +5798,7 @@
         <v>9: Fl G 4s</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -5847,7 +5859,7 @@
         <v>10: Fl R 4s</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -5905,7 +5917,7 @@
         <v>11: Q G</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -5966,7 +5978,7 @@
         <v>12: Fl G 4s</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -6027,7 +6039,7 @@
         <v>13: Fl G 4s</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -6088,7 +6100,7 @@
         <v>14: Fl R 4s</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -6146,7 +6158,7 @@
         <v>15: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -6207,7 +6219,7 @@
         <v>16: Fl G 2.5s</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -6265,7 +6277,7 @@
         <v>17: Fl R 4s</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -6323,7 +6335,7 @@
         <v>18: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5</v>
       </c>
@@ -6381,7 +6393,7 @@
         <v>19: Fl R 4s</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -6442,7 +6454,7 @@
         <v>20: Fl G 4s</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>5</v>
       </c>
@@ -6503,7 +6515,7 @@
         <v>21: Fl W 4s</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -6564,7 +6576,7 @@
         <v>22: Fl G 4s</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -6625,7 +6637,7 @@
         <v>23: Fl G 4s</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -6686,7 +6698,7 @@
         <v>24: Fl R 4s</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
@@ -6747,7 +6759,7 @@
         <v>25: Fl R 4s</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -6808,7 +6820,7 @@
         <v>26: Fl G 4s</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
@@ -6869,7 +6881,7 @@
         <v>27: Fl G 4s</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4</v>
       </c>
@@ -6930,7 +6942,7 @@
         <v>28: Fl R 4s</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4</v>
       </c>
@@ -6991,7 +7003,7 @@
         <v>29: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -7052,7 +7064,7 @@
         <v>30: Fl G 2.5s</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -7113,7 +7125,7 @@
         <v>31: Q G</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -7174,7 +7186,7 @@
         <v>32: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -7235,7 +7247,7 @@
         <v>33: Fl G 4s</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -7296,7 +7308,7 @@
         <v>34: Fl R 6s</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -7357,7 +7369,7 @@
         <v>35: Fl R 4s</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4</v>
       </c>
@@ -7418,7 +7430,7 @@
         <v>36: Fl G 4s</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -7479,7 +7491,7 @@
         <v>37: Fl G 2.5s</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -7540,7 +7552,7 @@
         <v>38: Fl Y 2.5s</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -7601,7 +7613,7 @@
         <v>39: Fl G 4s</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>4</v>
       </c>
@@ -7662,7 +7674,7 @@
         <v>40: Fl G 4s</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4</v>
       </c>
@@ -7723,7 +7735,7 @@
         <v>41: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4</v>
       </c>
@@ -7784,7 +7796,7 @@
         <v>42: Fl R 6s</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>4</v>
       </c>
@@ -7845,7 +7857,7 @@
         <v>43: Fl G 2.5s</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -7906,7 +7918,7 @@
         <v>44: Fl R 4s</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>4</v>
       </c>
@@ -7967,7 +7979,7 @@
         <v>45: Fl R 4s</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>4</v>
       </c>
@@ -8028,7 +8040,7 @@
         <v>46: Fl G 2.5s</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4</v>
       </c>
@@ -8089,7 +8101,7 @@
         <v>47: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4</v>
       </c>
@@ -8150,7 +8162,7 @@
         <v>48: Fl R 4s</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -8211,7 +8223,7 @@
         <v>49: Fl G 4s</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>4</v>
       </c>
@@ -8272,7 +8284,7 @@
         <v>50: Fl R 4s</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>4</v>
       </c>
@@ -8333,7 +8345,7 @@
         <v>51: Fl R 4s</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>4</v>
       </c>
@@ -8394,7 +8406,7 @@
         <v>52: Fl G 4s</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>4</v>
       </c>
@@ -8455,7 +8467,7 @@
         <v>53: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>4</v>
       </c>
@@ -8516,7 +8528,7 @@
         <v>54: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4</v>
       </c>
@@ -8577,7 +8589,7 @@
         <v>55: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4</v>
       </c>
@@ -8641,7 +8653,7 @@
         <v>56: Fl R 4s</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>4</v>
       </c>
@@ -8702,7 +8714,7 @@
         <v>57: Fl G 4s</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4</v>
       </c>
@@ -8763,7 +8775,7 @@
         <v>58: Fl (2+1)R 6s</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4</v>
       </c>
@@ -8824,7 +8836,7 @@
         <v>59: Fl G 4s</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>4</v>
       </c>
@@ -8885,7 +8897,7 @@
         <v>60: Fl G 2.5s</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>4</v>
       </c>
@@ -8946,7 +8958,7 @@
         <v>61: Fl R 4s</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>4</v>
       </c>
@@ -9007,7 +9019,7 @@
         <v>62: Fl G 2.5s</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>4</v>
       </c>
@@ -9068,7 +9080,7 @@
         <v>63: Fl G 4s</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>4</v>
       </c>
@@ -9129,7 +9141,7 @@
         <v>64: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>4</v>
       </c>
@@ -9190,7 +9202,7 @@
         <v>65: Fl R 4s</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>4</v>
       </c>
@@ -9251,7 +9263,7 @@
         <v>66: Fl R 4s</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>4</v>
       </c>
@@ -9312,7 +9324,7 @@
         <v>67: Fl G 4s</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>4</v>
       </c>
@@ -9373,7 +9385,7 @@
         <v>68: Q R</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>4</v>
       </c>
@@ -9434,7 +9446,7 @@
         <v>69: Q G</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>4</v>
       </c>
@@ -9495,7 +9507,7 @@
         <v>70: Fl G 4s</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>4</v>
       </c>
@@ -9556,7 +9568,7 @@
         <v>71: Fl R 4s</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>4</v>
       </c>
@@ -9620,7 +9632,7 @@
         <v>72: Fl G 4s</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>4</v>
       </c>
@@ -9681,7 +9693,7 @@
         <v>73: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>4</v>
       </c>
@@ -9742,7 +9754,7 @@
         <v>74: Q R</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>4</v>
       </c>
@@ -9803,7 +9815,7 @@
         <v>75: Fl G 2.5s</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>4</v>
       </c>
@@ -9864,7 +9876,7 @@
         <v>76: Q G</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>4</v>
       </c>
@@ -9925,7 +9937,7 @@
         <v>77: Fl R 4s</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>4</v>
       </c>
@@ -9986,7 +9998,7 @@
         <v>78: Fl (2+1)G 6s</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>4</v>
       </c>
@@ -10047,7 +10059,7 @@
         <v>79: Fl G 4s</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>4</v>
       </c>
@@ -10108,7 +10120,7 @@
         <v>80: Fl G 4s</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>4</v>
       </c>
@@ -10169,7 +10181,7 @@
         <v>81: Fl G 4s</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>4</v>
       </c>
@@ -10230,7 +10242,7 @@
         <v>82: Fl R 4s</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>4</v>
       </c>
@@ -10291,7 +10303,7 @@
         <v>83: Fl R 4s</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>4</v>
       </c>
@@ -10352,7 +10364,7 @@
         <v>84: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>4</v>
       </c>
@@ -10413,7 +10425,7 @@
         <v>85: Fl G 4s</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>4</v>
       </c>
@@ -10474,7 +10486,7 @@
         <v>86: Fl R 4s</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>4</v>
       </c>
@@ -10535,7 +10547,7 @@
         <v>87: Fl G 4s</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>3</v>
       </c>
@@ -10596,7 +10608,7 @@
         <v>88: Q G</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>3</v>
       </c>
@@ -10657,7 +10669,7 @@
         <v>89: Q G</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>3</v>
       </c>
@@ -10718,7 +10730,7 @@
         <v>90: Fl R 4s</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>3</v>
       </c>
@@ -10779,7 +10791,7 @@
         <v>91: Q G</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>3</v>
       </c>
@@ -10840,7 +10852,7 @@
         <v>92: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>3</v>
       </c>
@@ -10901,7 +10913,7 @@
         <v>93: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>3</v>
       </c>
@@ -10962,7 +10974,7 @@
         <v>94: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>3</v>
       </c>
@@ -11023,7 +11035,7 @@
         <v>95: Q G</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>3</v>
       </c>
@@ -11084,7 +11096,7 @@
         <v>96: Fl R 4s</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>3</v>
       </c>
@@ -11145,7 +11157,7 @@
         <v>97: Q G</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>3</v>
       </c>
@@ -11209,7 +11221,7 @@
         <v>98: Fl R 4s</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>3</v>
       </c>
@@ -11270,7 +11282,7 @@
         <v>99: Fl G 4s</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>3</v>
       </c>
@@ -11331,7 +11343,7 @@
         <v>100: Fl G 4s</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>3</v>
       </c>
@@ -11392,7 +11404,7 @@
         <v>101: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>3</v>
       </c>
@@ -11453,7 +11465,7 @@
         <v>102: Fl R 4s</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>3</v>
       </c>
@@ -11514,7 +11526,7 @@
         <v>103: Fl R 4s</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0</v>
       </c>
@@ -11575,7 +11587,7 @@
         <v>104: Q W</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0</v>
       </c>
@@ -11636,7 +11648,7 @@
         <v>105: Fl R 4s</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0</v>
       </c>
@@ -11697,7 +11709,7 @@
         <v>106: Fl G 4s</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0</v>
       </c>
@@ -11758,7 +11770,7 @@
         <v>107: Fl R 4s</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0</v>
       </c>
@@ -11819,7 +11831,7 @@
         <v>108: Q R</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0</v>
       </c>
@@ -11880,7 +11892,7 @@
         <v>109: Q G</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0</v>
       </c>
@@ -11941,7 +11953,7 @@
         <v>110: Q R</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0</v>
       </c>
@@ -12002,7 +12014,7 @@
         <v>111: Q G</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0</v>
       </c>
@@ -12063,7 +12075,7 @@
         <v>112: Q R</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0</v>
       </c>
@@ -12124,7 +12136,7 @@
         <v>113: Q G</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0</v>
       </c>
@@ -12185,7 +12197,7 @@
         <v>114: F Y</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>0</v>
       </c>
@@ -12243,7 +12255,7 @@
         <v>115: Fl Y 4s</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0</v>
       </c>
@@ -12304,7 +12316,7 @@
         <v>116: F Y</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0</v>
       </c>
@@ -12365,7 +12377,7 @@
         <v>117: Q R</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0</v>
       </c>
@@ -12426,7 +12438,7 @@
         <v>118: Q G</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>0</v>
       </c>
@@ -12487,7 +12499,7 @@
         <v>119: Fl W 10s</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>0</v>
       </c>
@@ -12545,7 +12557,7 @@
         <v>120: Fl Y 4s</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>0</v>
       </c>
@@ -12606,7 +12618,7 @@
         <v>121: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>0</v>
       </c>
@@ -12667,7 +12679,7 @@
         <v>122: Fl G 2.5s</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>0</v>
       </c>
@@ -12728,7 +12740,7 @@
         <v>123: Fl R 4s</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0</v>
       </c>
@@ -12789,7 +12801,7 @@
         <v>124: Fl G 4s</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>0</v>
       </c>
@@ -12850,7 +12862,7 @@
         <v>125: Fl G 4s</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>0</v>
       </c>
@@ -12911,7 +12923,7 @@
         <v>126: Q R</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>0</v>
       </c>
@@ -12972,7 +12984,7 @@
         <v>127: Fl R 2.5s</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>0</v>
       </c>
@@ -13033,7 +13045,7 @@
         <v>128: Fl G 4s</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>0</v>
       </c>
@@ -13094,7 +13106,7 @@
         <v>129: Fl R 4s</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>0</v>
       </c>
@@ -13152,7 +13164,7 @@
         <v>130: Fl Y 4s</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>0</v>
       </c>

</xml_diff>